<commit_message>
latest update on pdf crawler
</commit_message>
<xml_diff>
--- a/Data/archivoLinks.xlsx
+++ b/Data/archivoLinks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Innovación\SIFIC Crawler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboratorio\SIFIC_Crawler\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA05A80-72FA-457E-88CB-01B7AD78C13D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52A823E-A507-409C-A09B-62953F0EEDC4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="570" windowWidth="19440" windowHeight="15000" xr2:uid="{876FF047-1D07-4CC8-821E-16CED0CFC1C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{876FF047-1D07-4CC8-821E-16CED0CFC1C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1393,18 +1393,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0A2A5E-7C7D-415F-914D-69C21C4AE9E9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
     <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>